<commit_message>
update new official website
</commit_message>
<xml_diff>
--- a/output/scholars4dev.xlsx
+++ b/output/scholars4dev.xlsx
@@ -496,7 +496,7 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.ucl.ac.uk/scholarships/ucl-global-undergraduate-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Deadline:30 April 2022 (annual)</t>
+          <t>Deadline:30 April 2023 (annual)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -558,7 +558,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.uea.ac.uk/study/fees-and-funding/scholarships-finder/scholarships-a-z/international-development-full-fees-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -624,7 +624,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.nottingham.ac.uk/studywithus/international-applicants/scholarships-fees-and-finance/scholarships/masters-scholarships/dev-sol-masters.aspx</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -656,7 +656,11 @@
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -724,7 +728,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.sussex.ac.uk/study/fees-funding/masters-scholarships/view/1475-Chancellor-s-International-Scholarships</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -794,7 +798,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.cambridgetrust.org/scholarships/v-c-awards-and-cambridge-international-scholarships/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -864,7 +868,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://cscuk.fcdo.gov.uk/scholarships/commonwealth-shared-scholarships-applications/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -934,7 +938,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://cscuk.fcdo.gov.uk/scholarships/commonwealth-masters-scholarships/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -991,12 +995,12 @@
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr">
         <is>
-          <t>If you apply for a full- or part-time master’s or DPhil course at Oxford by the December or January deadline for your course, you will automatically be considered for a Clarendon Scholarship.You do not need to submit any additional documents specifically for the Clarendon Scholarships –there is no separate scholarship application form.   You do, however, need to apply before theDecember orJanuary deadline (6 or 20 January 2023) for your courseif you wish to be considered for the scholarship.</t>
+          <t>Applications are currently closed.</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.ox.ac.uk/clarendon</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -1062,7 +1066,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.ox.ac.uk/admissions/undergraduate/fees-and-funding/oxford-support/reach-oxford-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -1123,12 +1127,12 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>In order to be considered for this scholarship, you must select the Weidenfeld-Hoffman Scholarship and Leadership Programme in the Funding section of the University’s graduate application form and submit your application for graduate study by the relevant December or January deadline for your course(6 January or 20 January 2023). You must also complete a Weidenfeld-Hoffman Scholarships Statement and upload it together with your graduate application form, by the deadline.</t>
+          <t>Applications are currently closed.</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Weidenfeld Hoffman Trust Website:http://www.whtrust.org/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -1194,7 +1198,7 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.gatescambridge.org/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -1264,7 +1268,7 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:www.shu.ac.uk/transformtogether</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -1326,7 +1330,7 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.chevening.org/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -1396,7 +1400,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.rhodeshouse.ox.ac.uk/scholarships/applications/global/#apply-now</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -1466,7 +1470,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.scotland.org/study/saltire-scholarships</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -1536,7 +1540,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.studyinwales.ac.uk/global-wales-postgraduate-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -1602,7 +1606,7 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.ucl.ac.uk/scholarships/ucl-global-masters-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -1672,7 +1676,7 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.uwe.ac.uk/courses/funding/scholarships-and-bursaries/millennium-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -1738,7 +1742,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.ed.ac.uk/schools-departments/student-funding/postgraduate/international/medicine-vet-medicine/glenmore</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -1804,7 +1808,7 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.birmingham.ac.uk/international/students/global-masters-scholarship.aspx</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -1870,7 +1874,7 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.swansea.ac.uk/humanandhealthsciences/eira-francis-davies-scholarship/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -1936,7 +1940,7 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.gla.ac.uk/scholarships/universityofglasgowinternationalleadershipscholarship/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -2006,7 +2010,7 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.uwe.ac.uk/courses/funding/chancellors-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -2076,7 +2080,7 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.uwl.ac.uk/courses/undergraduate-study/fees-and-funding/bursaries-and-scholarships</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -2146,7 +2150,7 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.ucl.ac.uk/ioe/about-ioe/global-reach/scholarships-and-funding</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -2216,7 +2220,7 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.arts.ac.uk/study-at-ual/fees-and-funding/scholarships-search/ual-international-postgraduate-50,000-scholarships</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -2282,7 +2286,7 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.rotary.org/en/peace-fellowships</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -2344,7 +2348,7 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.sbs.ox.ac.uk/oxford-experience/scholarships-and-funding/oxford-pershing-square-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -2414,7 +2418,7 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.bath.ac.uk/campaigns/deans-award-for-academic-excellence-scholarship/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -2484,7 +2488,7 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.kent.ac.uk/scholarships/search/FN36ECODEV01</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -2554,7 +2558,7 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.ntu.ac.uk/international/scholarships-and-fees/scholarships</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -2620,7 +2624,7 @@
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.ed.ac.uk/student-funding/postgraduate/e-learning/glenmore-online</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -2686,7 +2690,7 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.ucl.ac.uk/scholarships/denys-holland-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -2752,7 +2756,7 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www1.uwe.ac.uk/students/feesandfunding/fundingandscholarships/internationalstudentfunding/uweinternationalscholarships/postgraduatescholarships.aspx</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -2818,7 +2822,7 @@
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.lse.ac.uk/study-at-lse/Graduate/fees-and-funding/carsten-stoehr-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -2888,7 +2892,7 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.lse.ac.uk/study-at-lse/Graduate/fees-and-funding/lse-masters-awards</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -2958,7 +2962,7 @@
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.exeter.ac.uk/studying/funding/award/?id=3942</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -3028,7 +3032,7 @@
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.reading.ac.uk/apd/pg-taught/empoweringchangescholarship.aspx</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -3098,7 +3102,7 @@
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.emm-aces.org/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -3164,7 +3168,7 @@
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://skollscholarship.org/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -3234,7 +3238,7 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.marshallscholarship.org/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -3304,7 +3308,7 @@
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.dundee.ac.uk/scholarships/2020-21/uod-global-excellence-pg/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -3374,7 +3378,7 @@
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.surrey.ac.uk/fees-and-funding/scholarships-and-bursaries/women-leadership-scholarship-2020</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -3432,7 +3436,7 @@
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.coltfoundation.org.uk/phd-fellowships/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -3502,7 +3506,7 @@
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://london.ac.uk/applications/funding-your-study/scholarships-and-bursaries/varadi-scholarships#eligibility-19980</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -3572,7 +3576,7 @@
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.brad.ac.uk/scholarships/info/Professor-Rae-Earnshaw-Masters-Scholarship-2019</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -3642,7 +3646,7 @@
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.uea.ac.uk/study/fees-and-funding/scholarships-finder/scholarships-a-z/international-scholarship-schemes-4000</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -3712,7 +3716,7 @@
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www1.uwe.ac.uk/students/feesandfunding/fundingandscholarships/internationalstudentfunding/internationalscholarships/postgraduatescholarships.aspx</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -3782,7 +3786,7 @@
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.sussex.ac.uk/study/fees-funding/masters-scholarships/view/1118-Geoffrey-Oldham-Memorial-Scholarships</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -3852,7 +3856,7 @@
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.manchester.ac.uk/study/masters/funding/opportunity-search/display/?id=00000382&amp;offset=0&amp;sort=name&amp;sortdir=ascending&amp;subjectArea=&amp;nationality=&amp;submit=</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -3922,7 +3926,7 @@
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.ed.ac.uk/student-funding/postgraduate/international/other-funding/saltire</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -3992,7 +3996,7 @@
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.bath.ac.uk/campaigns/global-leaders-scholarship/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -4058,7 +4062,7 @@
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.westminster.ac.uk/study/fees-and-funding/scholarships/westminster-undergraduate-full-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -4128,7 +4132,7 @@
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.sheffield.ac.uk/international/fees-and-funding/scholarships/postgraduate/usas</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -4198,7 +4202,7 @@
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.exeter.ac.uk/postgraduate/money/fundingsearch/awarddetails/?id=3851</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -4264,7 +4268,7 @@
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.bradford.ac.uk/scholarships/info/Peace-Studies-and-International-Development-Scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -4330,7 +4334,7 @@
       </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.lshtm.ac.uk/study/fees-and-funding/funding-scholarships/2020-21-wellcome-trust-masters-studentship-msc-public-health</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -4400,7 +4404,7 @@
       </c>
       <c r="N59" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.cranfield.ac.uk/funding/funding-opportunities/international-water-association-and-cranfield-university-excellence-scholarships</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -4470,7 +4474,7 @@
       </c>
       <c r="N60" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.ids.ac.uk/learn-at-ids/get-funding/ids-graduate-scholarship-2020/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -4540,7 +4544,7 @@
       </c>
       <c r="N61" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.westminster.ac.uk/study/fees-and-funding/scholarships/short-course-nutrition-in-emergencies-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -4610,7 +4614,7 @@
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.dur.ac.uk/scholarships/lioness/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -4680,7 +4684,7 @@
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.york.ac.uk/study/undergraduate/fees-funding/international/scholarships/asylum-seekers-scholarship/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -4746,7 +4750,7 @@
       </c>
       <c r="N64" t="inlineStr">
         <is>
-          <t>Official Website:https://www.nottingham.ac.uk/pgstudy/funding/vc-scholarship-for-research-excellence-international</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -4816,7 +4820,7 @@
       </c>
       <c r="N65" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.dundee.ac.uk/study/scholarships/2020-21/humanitarian-scholarship/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -4882,7 +4886,7 @@
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.kcl.ac.uk/ghsm/postgraduate/scholarships</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -4952,7 +4956,7 @@
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.marshalpapworth.com/our-scholarships/scholarship-details/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -5022,7 +5026,7 @@
       </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.lancaster.ac.uk/arts-and-social-sciences/study/postgraduate/funding/fully-funded-research-scholarships/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -5088,7 +5092,7 @@
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.lse.ac.uk/study-at-lse/Graduate/fees-and-funding/Wellcome-Award-MSc-in-Health-and-International-Development</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -5154,7 +5158,7 @@
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.imperial.ac.uk/business-school/programmes/msc-climate-change/fees-and-funding/scholarships/#bseisu-imperial-college-london-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -5224,7 +5228,7 @@
       </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.lshtm.ac.uk/study/fees-and-funding/funding-scholarships/2020-21-wellcome-trust-doctoral-studentships</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -5294,7 +5298,7 @@
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://warwick.ac.uk/fac/sci/lifesci/study/pgt/funding/slsexcellencescholarships/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -5364,7 +5368,7 @@
       </c>
       <c r="N73" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://globed.eu/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -5430,7 +5434,7 @@
       </c>
       <c r="N74" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.ed.ac.uk/history-classics-archaeology/graduate-school/fees-funding/funding/phd/global</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -5496,7 +5500,7 @@
       </c>
       <c r="N75" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.stx.ox.ac.uk/prospective-students/funding-support/st-cross-worldwide-scholarships</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -5562,7 +5566,7 @@
       </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.westminster.ac.uk/study/fees-and-funding/scholarships/tony-shaw-international-students-house-ish-scholarships</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -5632,7 +5636,7 @@
       </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.bathspa.ac.uk/students/student-finance/scholarships-and-funding/international-office-scholarships/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -5698,7 +5702,7 @@
       </c>
       <c r="N78" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.opensocietyfoundations.org/grants/civil-society-leadership-awards</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -5764,7 +5768,7 @@
       </c>
       <c r="N79" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.westminster.ac.uk/study/fees-and-funding/scholarships/vice-chancellor-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -5830,7 +5834,7 @@
       </c>
       <c r="N80" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.ed.ac.uk/student-funding/postgraduate/e-learning/commglobalhealth</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -5896,7 +5900,7 @@
       </c>
       <c r="N81" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.imperial.ac.uk/study/pg/fees-and-funding/scholarships/presidents-phd-scholarships/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -5966,7 +5970,7 @@
       </c>
       <c r="N82" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.ucl.ac.uk/prospective-students/scholarships/undergraduate/access_opportunity_scholarship_folder</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -6032,7 +6036,7 @@
       </c>
       <c r="N83" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.bradford.ac.uk/scholarships/info/half-fee-2018-19</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -6102,7 +6106,7 @@
       </c>
       <c r="N84" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.lsbu.ac.uk/courses/postgraduate/fees-and-funding/scholarships/vice-chancellor-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -6168,7 +6172,7 @@
       </c>
       <c r="N85" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.coventry.ac.uk/international-students-hub/new-students/international-scholarships-and-discounts/international-scholarships/apply-for-a-scholarship-/future-global-leaders-scholarship/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -6238,7 +6242,7 @@
       </c>
       <c r="N86" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.essex.ac.uk/fees-and-funding/masters/scholarships/women-future.aspx</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -6304,7 +6308,7 @@
       </c>
       <c r="N87" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.bradford.ac.uk/fees-and-financial-support/university-scholarships-and-support/info/global-development-scholarship-2017-18</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -6374,7 +6378,7 @@
       </c>
       <c r="N88" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.exeter.ac.uk/postgraduate/money/fundingsearch/awarddetails/?id=2466</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -6440,7 +6444,7 @@
       </c>
       <c r="N89" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.westminster.ac.uk/study/prospective-students/fees-and-funding/scholarships/postgraduate-scholarships/disaster-regeneration-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -6510,7 +6514,7 @@
       </c>
       <c r="N90" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.arts.ac.uk/study-at-ual/student-fees–funding/scholarships-search/ual-vice-chancellors-postgraduate-international-scholarships/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -6576,7 +6580,7 @@
       </c>
       <c r="N91" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.westminster.ac.uk/study/prospective-students/fees-and-funding/scholarships/international-postgraduate-scholarships/westminster-full-fee-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -6646,7 +6650,7 @@
       </c>
       <c r="N92" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.soas.ac.uk/registry/scholarships/ferguson-scholarships.html</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -6716,7 +6720,7 @@
       </c>
       <c r="N93" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www1.uwe.ac.uk/bl/bbs/courses/mba/bristolmbascholarships.aspx</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -6782,7 +6786,7 @@
       </c>
       <c r="N94" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.roehampton.ac.uk/Courses/Graduate-School/Funding/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -6848,7 +6852,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.uwlinternationalscholarship.com/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -6914,7 +6918,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.ljmu.ac.uk/study/international-students/financing-your-study/scholarships</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -6980,7 +6984,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.westminster.ac.uk/study/prospective-students/fees-and-funding/scholarships/international-postgraduate-scholarships/cavendish-research-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -7050,7 +7054,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www1.uwe.ac.uk/students/feesandfunding/fundingandscholarships/internationalstudentfunding/uweinternationalscholarships/postgraduatescholarships.aspx</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -7120,7 +7124,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.see.leeds.ac.uk/admissions-and-study/masters-degrees/admissions-and-study/scholarships/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -7190,7 +7194,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.see.leeds.ac.uk/admissions-and-study/masters-degrees/admissions-and-study/scholarships/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -7260,7 +7264,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.see.leeds.ac.uk/admissions-and-study/masters-degrees/admissions-and-study/scholarships/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -7326,7 +7330,7 @@
       </c>
       <c r="N102" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.swansea.ac.uk/international/students/fees-and-funding/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -7388,7 +7392,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.lse.ac.uk/internationalDevelopment/programmeForAfricanLeadership/howtoapply.aspx?utm_source=Newsletter%20to%20universities&amp;utm_medium=email&amp;utm_campaign=Recruitment%202015%2F16%20-%20universities</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -7458,7 +7462,7 @@
       </c>
       <c r="N104" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www1.uwe.ac.uk/students/feesandfunding/fundingandscholarships/internationalstudentfunding/uweinternationalscholarships/postgraduatescholarships.aspx</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -7524,7 +7528,7 @@
       </c>
       <c r="N105" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.soas.ac.uk/registry/scholarships/the-cultures-of-resistance-scholarships.html</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -7594,7 +7598,7 @@
       </c>
       <c r="N106" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.ed.ac.uk/student-funding/postgraduate/international/global/health</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -7664,7 +7668,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.roehampton.ac.uk/Finance/Sacred-Heart-Scholarship-(RUSH)/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -7730,7 +7734,7 @@
       </c>
       <c r="N108" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:https://www.dur.ac.uk/scholarships/postgraduate/university/ruthfirst/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -7796,7 +7800,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.ed.ac.uk/schools-departments/student-funding/postgraduate/international/global/masters</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -7858,7 +7862,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.ox.ac.uk/admissions/graduate/fees-and-funding/graduate-scholarships/university-wide-scholarships/eldred-waverley-scholarship-linacre-college</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -7928,7 +7932,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.soas.ac.uk/gdai/gdai—ma-scholarships.html</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -7990,7 +7994,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.ox.ac.uk/admissions/graduate/fees-and-funding/graduate-scholarships/university-wide-scholarships/oppenheimer-fund-scholarships</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -8060,7 +8064,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.ed.ac.uk/schools-departments/student-funding/postgraduate/international/global/development</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -8130,7 +8134,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.nottingham.ac.uk/business/ma/scholarships.html</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -8200,7 +8204,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.ntu.ac.uk/sat/courses/fees_funding/171982.html</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -8258,7 +8262,7 @@
       <c r="M116" t="inlineStr"/>
       <c r="N116" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.swansea.ac.uk/international/students/fees-and-funding/scholarships/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -8312,7 +8316,7 @@
       <c r="M117" t="inlineStr"/>
       <c r="N117" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.nottingham.ac.uk/business/phd/Scholarships.html</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -8378,7 +8382,7 @@
       </c>
       <c r="N118" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.lboro.ac.uk/study/finance/international/informationfor/africa/</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -8444,7 +8448,7 @@
       </c>
       <c r="N119" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.westminster.ac.uk/study/prospective-students/fees-and-funding/scholarships/postgraduate-scholarships/african-education-scholarship</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>
@@ -8514,7 +8518,7 @@
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>Official Scholarship Website:http://www.ed.ac.uk/schools-departments/student-funding/postgraduate/international/region/southern-africa</t>
+          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update new data official site
</commit_message>
<xml_diff>
--- a/output/scholars4dev.xlsx
+++ b/output/scholars4dev.xlsx
@@ -496,7 +496,7 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -558,7 +558,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -624,7 +624,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -658,7 +658,7 @@
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -798,7 +798,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -868,7 +868,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -938,7 +938,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -1132,7 +1132,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -1198,7 +1198,7 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -1268,7 +1268,7 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -1540,7 +1540,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -1676,7 +1676,7 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -1808,7 +1808,7 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -2010,7 +2010,7 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -2080,7 +2080,7 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -2150,7 +2150,7 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -2220,7 +2220,7 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -2348,7 +2348,7 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -2418,7 +2418,7 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -2488,7 +2488,7 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -2558,7 +2558,7 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -2624,7 +2624,7 @@
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -2690,7 +2690,7 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -2756,7 +2756,7 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -2822,7 +2822,7 @@
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -2892,7 +2892,7 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -2962,7 +2962,7 @@
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -3032,7 +3032,7 @@
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -3102,7 +3102,7 @@
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -3168,7 +3168,7 @@
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -3238,7 +3238,7 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -3308,7 +3308,7 @@
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -3378,7 +3378,7 @@
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -3436,7 +3436,7 @@
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -3506,7 +3506,7 @@
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -3576,7 +3576,7 @@
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -3646,7 +3646,7 @@
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -3716,7 +3716,7 @@
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -3856,7 +3856,7 @@
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -3926,7 +3926,7 @@
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -3996,7 +3996,7 @@
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -4062,7 +4062,7 @@
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -4132,7 +4132,7 @@
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -4202,7 +4202,7 @@
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -4268,7 +4268,7 @@
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -4334,7 +4334,7 @@
       </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -4404,7 +4404,7 @@
       </c>
       <c r="N59" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -4474,7 +4474,7 @@
       </c>
       <c r="N60" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -4544,7 +4544,7 @@
       </c>
       <c r="N61" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -4614,7 +4614,7 @@
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -4684,7 +4684,7 @@
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -4750,7 +4750,7 @@
       </c>
       <c r="N64" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -4820,7 +4820,7 @@
       </c>
       <c r="N65" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -4956,7 +4956,7 @@
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -5026,7 +5026,7 @@
       </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -5092,7 +5092,7 @@
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -5158,7 +5158,7 @@
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -5228,7 +5228,7 @@
       </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -5298,7 +5298,7 @@
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -5368,7 +5368,7 @@
       </c>
       <c r="N73" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="N74" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -5500,7 +5500,7 @@
       </c>
       <c r="N75" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -5566,7 +5566,7 @@
       </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -5702,7 +5702,7 @@
       </c>
       <c r="N78" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -5768,7 +5768,7 @@
       </c>
       <c r="N79" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -5834,7 +5834,7 @@
       </c>
       <c r="N80" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -5900,7 +5900,7 @@
       </c>
       <c r="N81" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -5970,7 +5970,7 @@
       </c>
       <c r="N82" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -6036,7 +6036,7 @@
       </c>
       <c r="N83" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -6106,7 +6106,7 @@
       </c>
       <c r="N84" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -6172,7 +6172,7 @@
       </c>
       <c r="N85" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -6242,7 +6242,7 @@
       </c>
       <c r="N86" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -6308,7 +6308,7 @@
       </c>
       <c r="N87" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -6378,7 +6378,7 @@
       </c>
       <c r="N88" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -6444,7 +6444,7 @@
       </c>
       <c r="N89" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -6514,7 +6514,7 @@
       </c>
       <c r="N90" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -6580,7 +6580,7 @@
       </c>
       <c r="N91" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -6650,7 +6650,7 @@
       </c>
       <c r="N92" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -6720,7 +6720,7 @@
       </c>
       <c r="N93" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -6786,7 +6786,7 @@
       </c>
       <c r="N94" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -6852,7 +6852,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -6918,7 +6918,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -6984,7 +6984,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -7054,7 +7054,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -7124,7 +7124,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -7194,7 +7194,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -7264,7 +7264,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -7330,7 +7330,7 @@
       </c>
       <c r="N102" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -7392,7 +7392,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -7462,7 +7462,7 @@
       </c>
       <c r="N104" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -7528,7 +7528,7 @@
       </c>
       <c r="N105" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -7598,7 +7598,7 @@
       </c>
       <c r="N106" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -7668,7 +7668,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -7734,7 +7734,7 @@
       </c>
       <c r="N108" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -7800,7 +7800,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -7862,7 +7862,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -7932,7 +7932,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -7994,7 +7994,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -8064,7 +8064,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -8134,7 +8134,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -8204,7 +8204,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -8262,7 +8262,7 @@
       <c r="M116" t="inlineStr"/>
       <c r="N116" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -8316,7 +8316,7 @@
       <c r="M117" t="inlineStr"/>
       <c r="N117" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -8382,7 +8382,7 @@
       </c>
       <c r="N118" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -8448,7 +8448,7 @@
       </c>
       <c r="N119" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>
@@ -8518,7 +8518,7 @@
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>Liên hệ Tamian UK Ltd để được tư vấn học bổng du học Anh miễn phí &lt;a href='https://tamian.uk/contact-us/'&gt;https://tamian.uk/contact-us/&lt;/a&gt;k</t>
+          <t>https://tamian.uk/contact-us/</t>
         </is>
       </c>
     </row>

</xml_diff>